<commit_message>
Removed old files, fix for Digital Bulletin Board Image
</commit_message>
<xml_diff>
--- a/_templates/Digital-Bulletin-Board-With-OneDrive/data-files/board-inhalte.xlsx
+++ b/_templates/Digital-Bulletin-Board-With-OneDrive/data-files/board-inhalte.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23322"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="565" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7C01E86B-F9B3-4C02-9990-4ECDA44877CB}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobiashaas/git/peakboard-templates/_templates/Digital-Bulletin-Board-With-OneDrive/data-files/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639E7816-ED70-FF45-9B32-0AA913E95F20}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="30100" windowHeight="19760" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Daily menu" sheetId="4" r:id="rId1"/>
     <sheet name="News" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -134,14 +139,14 @@
     <t>Die neue Website ist live und sie gefällt uns ausgesprochen gut. Konntet ihr schon einen Blick drauf werfen? Vielen Dank an alle Beteiligten. Falls ihr noch Fehler auf der Seite findet, lasst es gerne das Marketing-Team wissen.</t>
   </si>
   <si>
-    <t>https://image.freepik.com/free-psd/website-design-your-business_24972-394.jpg</t>
+    <t>https://image.freepik.com/free-psd/business-promotion-corporate-web-banner-template_120329-1249.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -514,18 +519,18 @@
       <selection activeCell="H2" sqref="H2:H99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="51.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" customWidth="1"/>
-    <col min="4" max="4" width="39.85546875" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" customWidth="1"/>
-    <col min="7" max="8" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="51.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" customWidth="1"/>
+    <col min="4" max="4" width="39.83203125" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" customWidth="1"/>
+    <col min="7" max="8" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -554,7 +559,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>44102</v>
       </c>
@@ -583,7 +588,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>44103</v>
       </c>
@@ -612,7 +617,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>44104</v>
       </c>
@@ -641,7 +646,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>44105</v>
       </c>
@@ -670,7 +675,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>44106</v>
       </c>
@@ -699,7 +704,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>44107</v>
       </c>
@@ -728,7 +733,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>44108</v>
       </c>
@@ -757,7 +762,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>44109</v>
       </c>
@@ -786,7 +791,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>44110</v>
       </c>
@@ -815,7 +820,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>44111</v>
       </c>
@@ -844,7 +849,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>44112</v>
       </c>
@@ -873,7 +878,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>44113</v>
       </c>
@@ -902,7 +907,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>44114</v>
       </c>
@@ -931,7 +936,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>44115</v>
       </c>
@@ -960,7 +965,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>44116</v>
       </c>
@@ -989,7 +994,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>44117</v>
       </c>
@@ -1018,7 +1023,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>44118</v>
       </c>
@@ -1047,7 +1052,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>44119</v>
       </c>
@@ -1076,7 +1081,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>44120</v>
       </c>
@@ -1105,7 +1110,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>44121</v>
       </c>
@@ -1134,7 +1139,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>44122</v>
       </c>
@@ -1163,7 +1168,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>44123</v>
       </c>
@@ -1192,7 +1197,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>44124</v>
       </c>
@@ -1221,7 +1226,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>44125</v>
       </c>
@@ -1250,7 +1255,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>44126</v>
       </c>
@@ -1279,7 +1284,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>44127</v>
       </c>
@@ -1308,7 +1313,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>44128</v>
       </c>
@@ -1337,7 +1342,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>44129</v>
       </c>
@@ -1366,7 +1371,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>44130</v>
       </c>
@@ -1395,7 +1400,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>44131</v>
       </c>
@@ -1424,7 +1429,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>44132</v>
       </c>
@@ -1453,7 +1458,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>44133</v>
       </c>
@@ -1482,7 +1487,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>44134</v>
       </c>
@@ -1511,7 +1516,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>44135</v>
       </c>
@@ -1540,7 +1545,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>44136</v>
       </c>
@@ -1569,7 +1574,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>44137</v>
       </c>
@@ -1598,7 +1603,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>44138</v>
       </c>
@@ -1627,7 +1632,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>44139</v>
       </c>
@@ -1656,7 +1661,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>44140</v>
       </c>
@@ -1685,7 +1690,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>44141</v>
       </c>
@@ -1714,7 +1719,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>44142</v>
       </c>
@@ -1743,7 +1748,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>44143</v>
       </c>
@@ -1772,7 +1777,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>44144</v>
       </c>
@@ -1801,7 +1806,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>44145</v>
       </c>
@@ -1830,7 +1835,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>44146</v>
       </c>
@@ -1859,7 +1864,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>44147</v>
       </c>
@@ -1888,7 +1893,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>44148</v>
       </c>
@@ -1917,7 +1922,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>44149</v>
       </c>
@@ -1946,7 +1951,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>44150</v>
       </c>
@@ -1975,7 +1980,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>44151</v>
       </c>
@@ -2004,7 +2009,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>44152</v>
       </c>
@@ -2033,7 +2038,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>44153</v>
       </c>
@@ -2062,7 +2067,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>44154</v>
       </c>
@@ -2091,7 +2096,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>44155</v>
       </c>
@@ -2120,7 +2125,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>44156</v>
       </c>
@@ -2149,7 +2154,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>44157</v>
       </c>
@@ -2178,7 +2183,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>44158</v>
       </c>
@@ -2207,7 +2212,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>44159</v>
       </c>
@@ -2236,7 +2241,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>44160</v>
       </c>
@@ -2265,7 +2270,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>44161</v>
       </c>
@@ -2294,7 +2299,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>44162</v>
       </c>
@@ -2323,7 +2328,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>44163</v>
       </c>
@@ -2352,7 +2357,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>44164</v>
       </c>
@@ -2381,7 +2386,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>44165</v>
       </c>
@@ -2410,7 +2415,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>44166</v>
       </c>
@@ -2439,7 +2444,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>44167</v>
       </c>
@@ -2468,7 +2473,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>44168</v>
       </c>
@@ -2497,7 +2502,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>44169</v>
       </c>
@@ -2526,7 +2531,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>44170</v>
       </c>
@@ -2555,7 +2560,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>44171</v>
       </c>
@@ -2584,7 +2589,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>44172</v>
       </c>
@@ -2613,7 +2618,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>44173</v>
       </c>
@@ -2642,7 +2647,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="74" spans="1:9">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>44174</v>
       </c>
@@ -2671,7 +2676,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="75" spans="1:9">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>44175</v>
       </c>
@@ -2700,7 +2705,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>44176</v>
       </c>
@@ -2729,7 +2734,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>44177</v>
       </c>
@@ -2758,7 +2763,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>44178</v>
       </c>
@@ -2787,7 +2792,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>44179</v>
       </c>
@@ -2816,7 +2821,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>44180</v>
       </c>
@@ -2845,7 +2850,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>44181</v>
       </c>
@@ -2874,7 +2879,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="82" spans="1:9">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>44182</v>
       </c>
@@ -2903,7 +2908,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="83" spans="1:9">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>44183</v>
       </c>
@@ -2932,7 +2937,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>44184</v>
       </c>
@@ -2961,7 +2966,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="85" spans="1:9">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>44185</v>
       </c>
@@ -2990,7 +2995,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="86" spans="1:9">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>44186</v>
       </c>
@@ -3019,7 +3024,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="87" spans="1:9">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>44187</v>
       </c>
@@ -3048,7 +3053,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="88" spans="1:9">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>44188</v>
       </c>
@@ -3077,7 +3082,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="89" spans="1:9">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>44189</v>
       </c>
@@ -3106,7 +3111,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>44190</v>
       </c>
@@ -3135,7 +3140,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="91" spans="1:9">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>44191</v>
       </c>
@@ -3164,7 +3169,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="92" spans="1:9">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>44192</v>
       </c>
@@ -3193,7 +3198,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="93" spans="1:9">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>44193</v>
       </c>
@@ -3222,7 +3227,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="94" spans="1:9">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>44194</v>
       </c>
@@ -3251,7 +3256,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="95" spans="1:9">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>44195</v>
       </c>
@@ -3280,7 +3285,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="96" spans="1:9">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>44196</v>
       </c>
@@ -3309,7 +3314,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="97" spans="1:9">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>44197</v>
       </c>
@@ -3338,7 +3343,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="98" spans="1:9">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>44198</v>
       </c>
@@ -3367,7 +3372,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="99" spans="1:9">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>44199</v>
       </c>
@@ -3409,16 +3414,16 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="71.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="47.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="45.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="71.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="47.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61.83203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3435,7 +3440,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="60">
+    <row r="2" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>44083</v>
       </c>
@@ -3452,7 +3457,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="60">
+    <row r="3" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>44084</v>
       </c>
@@ -3469,7 +3474,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="60">
+    <row r="4" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>44085</v>
       </c>
@@ -3486,7 +3491,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="90">
+    <row r="5" spans="1:5" ht="80" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>44086</v>
       </c>
@@ -3503,7 +3508,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="45">
+    <row r="6" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>44087</v>
       </c>
@@ -3520,27 +3525,27 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="3"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
     </row>
   </sheetData>
@@ -3552,9 +3557,8 @@
     <hyperlink ref="E3" r:id="rId5" xr:uid="{87FF3097-E296-425D-877A-618163327E34}"/>
     <hyperlink ref="E4" r:id="rId6" xr:uid="{5D15FFAB-F62D-4191-9D64-53BC9AC6FB33}"/>
     <hyperlink ref="E5" r:id="rId7" xr:uid="{B8B1802E-E562-4DD9-A048-17666FE97206}"/>
-    <hyperlink ref="E6" r:id="rId8" xr:uid="{8052B891-6C2D-4D4B-9658-860CD6736702}"/>
-    <hyperlink ref="D6" r:id="rId9" display="'https://peakboard.com/?utm_source=dashboard&amp;utm_medium=peakboard&amp;utm_campaign=bulleting-board" xr:uid="{2EC656CC-9520-45D4-A771-A487292BD4C9}"/>
-    <hyperlink ref="D2" r:id="rId10" display="'https://peakboard.com/?utm_source=dashboard&amp;utm_medium=peakboard&amp;utm_campaign=bulleting-board" xr:uid="{2819221C-0983-44CD-B63A-122C44FAB9A8}"/>
+    <hyperlink ref="D6" r:id="rId8" display="'https://peakboard.com/?utm_source=dashboard&amp;utm_medium=peakboard&amp;utm_campaign=bulleting-board" xr:uid="{2EC656CC-9520-45D4-A771-A487292BD4C9}"/>
+    <hyperlink ref="D2" r:id="rId9" display="'https://peakboard.com/?utm_source=dashboard&amp;utm_medium=peakboard&amp;utm_campaign=bulleting-board" xr:uid="{2819221C-0983-44CD-B63A-122C44FAB9A8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>